<commit_message>
fixing some blend modes
</commit_message>
<xml_diff>
--- a/blend ´mode calcs check.xlsx
+++ b/blend ´mode calcs check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\TPM-FX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C1B1B4-F5CF-4ECF-A5D5-38096591EF56}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA6153D-A59F-4EA6-BAAE-118B2F57FD30}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6386" yWindow="1423" windowWidth="20263" windowHeight="14888" xr2:uid="{B3BDF030-FFC4-4FAB-975D-0B536C098592}"/>
+    <workbookView xWindow="19380" yWindow="2391" windowWidth="13534" windowHeight="15678" xr2:uid="{B3BDF030-FFC4-4FAB-975D-0B536C098592}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,11 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -60,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Bot Layer</t>
   </si>
@@ -126,6 +131,15 @@
   </si>
   <si>
     <t>Exclusion</t>
+  </si>
+  <si>
+    <t>HARD MIX</t>
+  </si>
+  <si>
+    <t>a&lt;1-b</t>
+  </si>
+  <si>
+    <t>1&gt;1-b</t>
   </si>
 </sst>
 </file>
@@ -490,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020A39F2-BFC3-4940-AF3C-A2E03E9C02A7}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -532,30 +546,30 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="D2">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="E2">
         <f>C2/255</f>
-        <v>0.19607843137254902</v>
+        <v>0.78431372549019607</v>
       </c>
       <c r="F2">
         <f>D2/255</f>
-        <v>0.94117647058823528</v>
+        <v>0.78431372549019607</v>
       </c>
       <c r="G2">
         <f>255-(255-D2)*(255-C2)/255</f>
-        <v>242.94117647058823</v>
+        <v>243.13725490196077</v>
       </c>
       <c r="I2">
         <f>J2*255</f>
-        <v>242.94117647058823</v>
+        <v>243.1372549019608</v>
       </c>
       <c r="J2">
         <f>1-(1-F2)*(1-E2)</f>
-        <v>0.9527104959630911</v>
+        <v>0.95347943098808152</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
@@ -563,30 +577,32 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <f>C2</f>
+        <v>200</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <f>D2</f>
+        <v>200</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E29" si="0">C3/255</f>
-        <v>3.9215686274509803E-2</v>
+        <f t="shared" ref="E3:E34" si="0">C3/255</f>
+        <v>0.78431372549019607</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F29" si="1">D3/255</f>
-        <v>0.19607843137254902</v>
+        <f t="shared" ref="F3:F34" si="1">D3/255</f>
+        <v>0.78431372549019607</v>
       </c>
       <c r="G3">
         <f>255*C3/(255-D3)</f>
-        <v>12.439024390243903</v>
+        <v>927.27272727272725</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I29" si="2">J3*255</f>
-        <v>12.439024390243901</v>
+        <v>927.27272727272725</v>
       </c>
       <c r="J3">
         <f>E3/(1-F3)</f>
-        <v>4.8780487804878044E-2</v>
+        <v>3.6363636363636362</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -594,30 +610,32 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <f>C2</f>
+        <v>200</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <f>D3</f>
+        <v>200</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>1.9607843137254902E-2</v>
+        <v>0.78431372549019607</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.78431372549019607</v>
       </c>
       <c r="G7">
         <f>C7*D7/255</f>
-        <v>0</v>
+        <v>156.86274509803923</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>156.8627450980392</v>
       </c>
       <c r="J7">
         <f>F7*E7</f>
-        <v>0</v>
+        <v>0.61514801999231061</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
@@ -625,9 +643,11 @@
         <v>9</v>
       </c>
       <c r="C11">
+        <f>C2</f>
         <v>200</v>
       </c>
       <c r="D11">
+        <f>D3</f>
         <v>200</v>
       </c>
       <c r="E11">
@@ -640,6 +660,10 @@
       </c>
       <c r="G11">
         <f>255 - ( ((255-C11)/D11)*255)</f>
+        <v>184.875</v>
+      </c>
+      <c r="H11">
+        <f xml:space="preserve"> 255 - ((255-C11)/D11 * 255)</f>
         <v>184.875</v>
       </c>
       <c r="I11">
@@ -682,30 +706,32 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>150</v>
+        <f>C2</f>
+        <v>200</v>
       </c>
       <c r="D15">
-        <v>150</v>
+        <f>D3</f>
+        <v>200</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0.58823529411764708</v>
+        <v>0.78431372549019607</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>0.58823529411764708</v>
+        <v>0.78431372549019607</v>
       </c>
       <c r="G15">
         <f>C15+D15-255</f>
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>45.000000000000007</v>
+        <v>145</v>
       </c>
       <c r="J15">
         <f>E15+F15-1</f>
-        <v>0.17647058823529416</v>
+        <v>0.56862745098039214</v>
       </c>
       <c r="L15" t="s">
         <v>12</v>
@@ -970,6 +996,83 @@
       <c r="I29">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33">
+        <v>200</v>
+      </c>
+      <c r="D33">
+        <v>200</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0.78431372549019607</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0.78431372549019607</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34">
+        <v>200</v>
+      </c>
+      <c r="D34">
+        <v>200</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0.78431372549019607</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0.78431372549019607</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>